<commit_message>
Fix the mismatch between entity classes and database field types, fix some auto-filling fields, and complete the test of adding, deleting and changing users and excel importing users
</commit_message>
<xml_diff>
--- a/src/main/resources/功能模块-数据库设计.xlsx
+++ b/src/main/resources/功能模块-数据库设计.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\junior year second\综合课程设计\文档大全\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\学习资料\学科\大三\实训\ComputerRoomManagement\ComputerRoomMangement-Backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DF6A7C-1B61-4528-AEA6-A775ABDE479F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577AC55D-FD4F-41D7-A551-1B1B43329E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1EB6AB7C-C387-4735-9BC6-648BE9AC4ABD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{1EB6AB7C-C387-4735-9BC6-648BE9AC4ABD}"/>
   </bookViews>
   <sheets>
     <sheet name="功能模块" sheetId="2" r:id="rId1"/>
     <sheet name="数据库" sheetId="1" r:id="rId2"/>
+    <sheet name="导入用户模板" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="183">
   <si>
     <t>账户：account</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -753,6 +754,10 @@
   </si>
   <si>
     <t>更新时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admain</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -799,7 +804,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -821,6 +826,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -971,7 +982,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1037,21 +1048,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1061,6 +1072,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1070,26 +1084,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1444,7 +1440,7 @@
       <c r="A2" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>90</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -1457,8 +1453,8 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="26" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="25" t="s">
         <v>92</v>
       </c>
       <c r="D3" s="10" t="s">
@@ -1468,8 +1464,8 @@
     </row>
     <row r="4" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="13" t="s">
         <v>94</v>
       </c>
@@ -1477,10 +1473,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>96</v>
       </c>
       <c r="D5" s="14" t="s">
@@ -1490,8 +1486,8 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="12" t="s">
         <v>98</v>
       </c>
@@ -1499,8 +1495,8 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="29" t="s">
+      <c r="B7" s="28"/>
+      <c r="C7" s="27" t="s">
         <v>99</v>
       </c>
       <c r="D7" s="14" t="s">
@@ -1510,8 +1506,8 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="29"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="14" t="s">
         <v>101</v>
       </c>
@@ -1519,8 +1515,8 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="26" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="25" t="s">
         <v>102</v>
       </c>
       <c r="D9" s="14" t="s">
@@ -1530,8 +1526,8 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="14" t="s">
         <v>104</v>
       </c>
@@ -1539,10 +1535,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>166</v>
       </c>
       <c r="D11" s="14" t="s">
@@ -1552,8 +1548,8 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="14" t="s">
         <v>106</v>
       </c>
@@ -1561,7 +1557,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
-      <c r="B13" s="27"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="13" t="s">
         <v>167</v>
       </c>
@@ -1572,7 +1568,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
-      <c r="B14" s="27"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="13" t="s">
         <v>168</v>
       </c>
@@ -1582,8 +1578,8 @@
       <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="13" t="s">
         <v>169</v>
       </c>
@@ -1596,7 +1592,7 @@
       <c r="A16" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="25" t="s">
         <v>111</v>
       </c>
       <c r="C16" s="21" t="s">
@@ -1609,8 +1605,8 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="26" t="s">
+      <c r="B17" s="28"/>
+      <c r="C17" s="25" t="s">
         <v>113</v>
       </c>
       <c r="D17" s="14" t="s">
@@ -1620,8 +1616,8 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="14" t="s">
         <v>115</v>
       </c>
@@ -1629,10 +1625,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="25" t="s">
         <v>117</v>
       </c>
       <c r="D19" s="14" t="s">
@@ -1642,8 +1638,8 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="10" t="s">
         <v>119</v>
       </c>
@@ -1651,7 +1647,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="24"/>
-      <c r="B21" s="28"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="12" t="s">
         <v>120</v>
       </c>
@@ -1662,10 +1658,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="24"/>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="25" t="s">
         <v>123</v>
       </c>
       <c r="D22" s="14" t="s">
@@ -1677,8 +1673,8 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="14" t="s">
         <v>126</v>
       </c>
@@ -1686,8 +1682,8 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="14" t="s">
         <v>127</v>
       </c>
@@ -1695,7 +1691,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
-      <c r="B25" s="27"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="14" t="s">
         <v>128</v>
       </c>
@@ -1706,8 +1702,8 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="26" t="s">
+      <c r="B26" s="28"/>
+      <c r="C26" s="25" t="s">
         <v>129</v>
       </c>
       <c r="D26" s="14" t="s">
@@ -1717,30 +1713,30 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="14" t="s">
         <v>131</v>
       </c>
       <c r="E27" s="11"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="14" t="s">
         <v>132</v>
       </c>
       <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="25" t="s">
         <v>135</v>
       </c>
       <c r="D29" s="14" t="s">
@@ -1751,17 +1747,17 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="28"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="26"/>
       <c r="D30" s="14" t="s">
         <v>138</v>
       </c>
       <c r="E30" s="11"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="14" t="s">
         <v>139</v>
       </c>
@@ -1773,8 +1769,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
-      <c r="B32" s="26" t="s">
+      <c r="A32" s="27"/>
+      <c r="B32" s="25" t="s">
         <v>142</v>
       </c>
       <c r="C32" s="14" t="s">
@@ -1786,8 +1782,8 @@
       <c r="E32" s="11"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="28"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="14" t="s">
         <v>144</v>
       </c>
@@ -1798,13 +1794,13 @@
       <c r="F33" s="16"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="C34" s="26" t="s">
+      <c r="C34" s="25" t="s">
         <v>147</v>
       </c>
       <c r="D34" s="13" t="s">
@@ -1813,9 +1809,9 @@
       <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
       <c r="D35" s="14" t="s">
         <v>149</v>
       </c>
@@ -1915,7 +1911,7 @@
       <c r="D50" s="19"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="26" t="s">
+      <c r="A51" s="25" t="s">
         <v>164</v>
       </c>
       <c r="B51" s="19" t="s">
@@ -1925,7 +1921,7 @@
       <c r="D51" s="19"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="28"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="19" t="s">
         <v>142</v>
       </c>
@@ -1942,24 +1938,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="A16:A28"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C26:C28"/>
     <mergeCell ref="A2:A15"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C3:C4"/>
@@ -1969,6 +1947,24 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="B11:B15"/>
     <mergeCell ref="C11:C12"/>
+    <mergeCell ref="A16:A28"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1979,8 +1975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D80F62-AD32-4D31-A959-DA3AC0FAD995}">
   <dimension ref="B2:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1999,42 +1995,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="35"/>
-      <c r="H2" s="33" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
+      <c r="H2" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="35"/>
-      <c r="N2" s="33" t="s">
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="36"/>
+      <c r="N2" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="36"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="36"/>
+      <c r="F3" s="33"/>
       <c r="H3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2047,7 +2043,7 @@
       <c r="K3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="36"/>
+      <c r="L3" s="33"/>
       <c r="N3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2060,22 +2056,22 @@
       <c r="Q3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="36"/>
+      <c r="R3" s="33"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="36"/>
+      <c r="F4" s="33"/>
       <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2088,7 +2084,7 @@
       <c r="K4" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="36"/>
+      <c r="L4" s="33"/>
       <c r="N4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2101,20 +2097,20 @@
       <c r="Q4" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="R4" s="36"/>
+      <c r="R4" s="33"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="36"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="33"/>
       <c r="H5" s="1" t="s">
         <v>39</v>
       </c>
@@ -2127,7 +2123,7 @@
       <c r="K5" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="36"/>
+      <c r="L5" s="33"/>
       <c r="N5" s="1" t="s">
         <v>39</v>
       </c>
@@ -2140,20 +2136,20 @@
       <c r="Q5" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="R5" s="36"/>
+      <c r="R5" s="33"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="33"/>
       <c r="H6" s="1" t="s">
         <v>41</v>
       </c>
@@ -2166,7 +2162,7 @@
       <c r="K6" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="36"/>
+      <c r="L6" s="33"/>
       <c r="N6" s="1" t="s">
         <v>60</v>
       </c>
@@ -2177,22 +2173,22 @@
         <v>63</v>
       </c>
       <c r="Q6" s="32"/>
-      <c r="R6" s="36"/>
+      <c r="R6" s="33"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="33"/>
       <c r="H7" s="1" t="s">
         <v>44</v>
       </c>
@@ -2203,7 +2199,7 @@
         <v>45</v>
       </c>
       <c r="K7" s="32"/>
-      <c r="L7" s="36"/>
+      <c r="L7" s="33"/>
       <c r="N7" s="4" t="s">
         <v>61</v>
       </c>
@@ -2217,19 +2213,19 @@
       <c r="R7" s="31"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" t="s">
         <v>174</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="33"/>
       <c r="H8" s="1" t="s">
         <v>46</v>
       </c>
@@ -2242,24 +2238,24 @@
       <c r="K8" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="L8" s="36"/>
+      <c r="L8" s="33"/>
       <c r="Q8" s="32"/>
       <c r="R8" s="32"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" t="s">
         <v>177</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="33"/>
       <c r="H9" s="4" t="s">
         <v>36</v>
       </c>
@@ -2277,44 +2273,44 @@
       <c r="R9" s="32"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" t="s">
         <v>179</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" t="s">
         <v>180</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="36"/>
-      <c r="N10" s="33" t="s">
+      <c r="E10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="N10" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="35"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="36"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="5" t="s">
         <v>181</v>
       </c>
       <c r="E11" s="30"/>
       <c r="F11" s="31"/>
-      <c r="H11" s="33" t="s">
+      <c r="H11" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="36"/>
       <c r="N11" s="1" t="s">
         <v>1</v>
       </c>
@@ -2327,14 +2323,9 @@
       <c r="Q11" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R11" s="36"/>
+      <c r="R11" s="33"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
       <c r="H12" s="1" t="s">
         <v>1</v>
       </c>
@@ -2347,7 +2338,7 @@
       <c r="K12" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="36"/>
+      <c r="L12" s="33"/>
       <c r="N12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2360,16 +2351,16 @@
       <c r="Q12" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="R12" s="36"/>
+      <c r="R12" s="33"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
       <c r="H13" s="1" t="s">
         <v>5</v>
       </c>
@@ -2382,7 +2373,7 @@
       <c r="K13" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="L13" s="36"/>
+      <c r="L13" s="33"/>
       <c r="N13" s="1" t="s">
         <v>19</v>
       </c>
@@ -2395,7 +2386,7 @@
       <c r="Q13" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="R13" s="36"/>
+      <c r="R13" s="33"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -2410,7 +2401,7 @@
       <c r="E14" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="36"/>
+      <c r="F14" s="33"/>
       <c r="H14" s="1" t="s">
         <v>51</v>
       </c>
@@ -2449,7 +2440,7 @@
       <c r="E15" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="36"/>
+      <c r="F15" s="33"/>
       <c r="H15" s="4" t="s">
         <v>52</v>
       </c>
@@ -2475,7 +2466,7 @@
       <c r="E16" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="36"/>
+      <c r="F16" s="33"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -2488,21 +2479,21 @@
         <v>22</v>
       </c>
       <c r="E17" s="32"/>
-      <c r="F17" s="36"/>
-      <c r="H17" s="33" t="s">
+      <c r="F17" s="33"/>
+      <c r="H17" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="35"/>
-      <c r="N17" s="33" t="s">
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="36"/>
+      <c r="N17" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="O17" s="34"/>
-      <c r="P17" s="34"/>
-      <c r="Q17" s="34"/>
-      <c r="R17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="36"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
@@ -2515,20 +2506,20 @@
         <v>21</v>
       </c>
       <c r="E18" s="32"/>
-      <c r="F18" s="36"/>
+      <c r="F18" s="33"/>
       <c r="H18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="39" t="s">
+      <c r="I18" t="s">
         <v>2</v>
       </c>
-      <c r="J18" s="39" t="s">
+      <c r="J18" t="s">
         <v>3</v>
       </c>
-      <c r="K18" s="40" t="s">
+      <c r="K18" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="L18" s="36"/>
+      <c r="L18" s="33"/>
       <c r="N18" s="1" t="s">
         <v>1</v>
       </c>
@@ -2541,7 +2532,7 @@
       <c r="Q18" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R18" s="36"/>
+      <c r="R18" s="33"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
@@ -2560,16 +2551,16 @@
       <c r="H19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="39" t="s">
+      <c r="I19" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="39" t="s">
+      <c r="J19" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="40" t="s">
+      <c r="K19" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="L19" s="36"/>
+      <c r="L19" s="33"/>
       <c r="N19" s="1" t="s">
         <v>5</v>
       </c>
@@ -2582,22 +2573,22 @@
       <c r="Q19" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="R19" s="36"/>
+      <c r="R19" s="33"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I20" s="39" t="s">
+      <c r="I20" t="s">
         <v>9</v>
       </c>
-      <c r="J20" s="39" t="s">
+      <c r="J20" t="s">
         <v>57</v>
       </c>
-      <c r="K20" s="40" t="s">
+      <c r="K20" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="L20" s="36"/>
+      <c r="L20" s="33"/>
       <c r="N20" s="1" t="s">
         <v>44</v>
       </c>
@@ -2608,29 +2599,29 @@
         <v>68</v>
       </c>
       <c r="Q20" s="32"/>
-      <c r="R20" s="36"/>
+      <c r="R20" s="33"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="36"/>
       <c r="H21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I21" s="39" t="s">
+      <c r="I21" t="s">
         <v>62</v>
       </c>
-      <c r="J21" s="39" t="s">
+      <c r="J21" t="s">
         <v>63</v>
       </c>
-      <c r="K21" s="40" t="s">
+      <c r="K21" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="L21" s="36"/>
+      <c r="L21" s="33"/>
       <c r="N21" s="4" t="s">
         <v>71</v>
       </c>
@@ -2658,20 +2649,20 @@
       <c r="E22" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="36"/>
+      <c r="F22" s="33"/>
       <c r="H22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I22" s="39" t="s">
+      <c r="I22" t="s">
         <v>62</v>
       </c>
-      <c r="J22" s="39" t="s">
+      <c r="J22" t="s">
         <v>64</v>
       </c>
-      <c r="K22" s="40" t="s">
+      <c r="K22" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="L22" s="36"/>
+      <c r="L22" s="33"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
@@ -2686,20 +2677,20 @@
       <c r="E23" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="36"/>
+      <c r="F23" s="33"/>
       <c r="H23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I23" s="39" t="s">
+      <c r="I23" t="s">
         <v>9</v>
       </c>
-      <c r="J23" s="39" t="s">
+      <c r="J23" t="s">
         <v>59</v>
       </c>
-      <c r="K23" s="40" t="s">
+      <c r="K23" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="L23" s="36"/>
+      <c r="L23" s="33"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
@@ -2714,18 +2705,18 @@
       <c r="E24" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="36"/>
-      <c r="H24" s="37" t="s">
+      <c r="F24" s="33"/>
+      <c r="H24" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I24" s="38" t="s">
+      <c r="I24" t="s">
         <v>179</v>
       </c>
-      <c r="J24" s="38" t="s">
+      <c r="J24" t="s">
         <v>180</v>
       </c>
-      <c r="K24" s="40"/>
-      <c r="L24" s="36"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="33"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
@@ -2740,14 +2731,14 @@
       <c r="E25" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="36"/>
-      <c r="H25" s="41" t="s">
+      <c r="F25" s="33"/>
+      <c r="H25" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="I25" s="42" t="s">
+      <c r="I25" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="J25" s="42" t="s">
+      <c r="J25" s="5" t="s">
         <v>181</v>
       </c>
       <c r="K25" s="30"/>
@@ -2764,7 +2755,7 @@
         <v>34</v>
       </c>
       <c r="E26" s="32"/>
-      <c r="F26" s="36"/>
+      <c r="F26" s="33"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
@@ -2782,121 +2773,121 @@
       <c r="F27" s="31"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="36"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="39" t="s">
+      <c r="D30" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="40" t="s">
+      <c r="E30" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="36"/>
+      <c r="F30" s="33"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="39" t="s">
+      <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="39" t="s">
+      <c r="D31" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="40" t="s">
+      <c r="E31" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="36"/>
+      <c r="F31" s="33"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="39" t="s">
+      <c r="C32" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="39" t="s">
+      <c r="D32" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="40" t="s">
+      <c r="E32" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="33"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="39" t="s">
+      <c r="C33" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="39" t="s">
+      <c r="D33" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="40" t="s">
+      <c r="E33" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="33"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="39" t="s">
+      <c r="C34" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="39" t="s">
+      <c r="D34" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="40"/>
-      <c r="F34" s="36"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="33"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="39" t="s">
+      <c r="C35" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="39" t="s">
+      <c r="D35" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="40"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C36" s="38" t="s">
+      <c r="C36" t="s">
         <v>179</v>
       </c>
-      <c r="D36" s="38" t="s">
+      <c r="D36" t="s">
         <v>180</v>
       </c>
-      <c r="E36" s="40"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="33"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C37" s="42" t="s">
+      <c r="C37" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="D37" s="42" t="s">
+      <c r="D37" s="5" t="s">
         <v>181</v>
       </c>
       <c r="E37" s="30"/>
@@ -2908,63 +2899,9 @@
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="N10:R10"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K19:L19"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="H17:L17"/>
@@ -2977,12 +2914,109 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="N10:R10"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A16CED-1914-426A-8275-7025C555F9C2}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="2">
+        <v>13456</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the field type of the database, complete the operation of the account and student
</commit_message>
<xml_diff>
--- a/src/main/resources/功能模块-数据库设计.xlsx
+++ b/src/main/resources/功能模块-数据库设计.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\学习资料\学科\大三\实训\ComputerRoomManagement\ComputerRoomMangement-Backend\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577AC55D-FD4F-41D7-A551-1B1B43329E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813EE221-45D8-4D69-91F3-33A9ADFEAF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{1EB6AB7C-C387-4735-9BC6-648BE9AC4ABD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{1EB6AB7C-C387-4735-9BC6-648BE9AC4ABD}"/>
   </bookViews>
   <sheets>
     <sheet name="功能模块" sheetId="2" r:id="rId1"/>
     <sheet name="数据库" sheetId="1" r:id="rId2"/>
     <sheet name="导入用户模板" sheetId="3" r:id="rId3"/>
+    <sheet name="导入学生模板" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="187">
   <si>
     <t>账户：account</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -758,6 +759,22 @@
   </si>
   <si>
     <t>admain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bigint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参照机房主键</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张三</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>202011班</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1042,49 +1059,49 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1404,7 +1421,7 @@
   <dimension ref="A1:H77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1437,10 +1454,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="27" t="s">
         <v>90</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -1452,9 +1469,9 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="28"/>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="27" t="s">
         <v>92</v>
       </c>
       <c r="D3" s="10" t="s">
@@ -1463,20 +1480,20 @@
       <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="13" t="s">
         <v>94</v>
       </c>
       <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="27" t="s">
         <v>96</v>
       </c>
       <c r="D5" s="14" t="s">
@@ -1485,18 +1502,18 @@
       <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="28"/>
-      <c r="C6" s="26"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="12" t="s">
         <v>98</v>
       </c>
       <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="28"/>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="30" t="s">
         <v>99</v>
       </c>
       <c r="D7" s="14" t="s">
@@ -1505,18 +1522,18 @@
       <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="28"/>
-      <c r="C8" s="27"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="14" t="s">
         <v>101</v>
       </c>
       <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="28"/>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="27" t="s">
         <v>102</v>
       </c>
       <c r="D9" s="14" t="s">
@@ -1525,20 +1542,20 @@
       <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="14" t="s">
         <v>104</v>
       </c>
       <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25" t="s">
+      <c r="A11" s="25"/>
+      <c r="B11" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="27" t="s">
         <v>166</v>
       </c>
       <c r="D11" s="14" t="s">
@@ -1547,16 +1564,16 @@
       <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="28"/>
-      <c r="C12" s="26"/>
+      <c r="C12" s="29"/>
       <c r="D12" s="14" t="s">
         <v>106</v>
       </c>
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="28"/>
       <c r="C13" s="13" t="s">
         <v>167</v>
@@ -1567,7 +1584,7 @@
       <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="28"/>
       <c r="C14" s="13" t="s">
         <v>168</v>
@@ -1578,8 +1595,8 @@
       <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="13" t="s">
         <v>169</v>
       </c>
@@ -1589,10 +1606,10 @@
       <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="27" t="s">
         <v>111</v>
       </c>
       <c r="C16" s="21" t="s">
@@ -1604,9 +1621,9 @@
       <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="28"/>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="27" t="s">
         <v>113</v>
       </c>
       <c r="D17" s="14" t="s">
@@ -1615,20 +1632,20 @@
       <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="14" t="s">
         <v>115</v>
       </c>
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25" t="s">
+      <c r="A19" s="25"/>
+      <c r="B19" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="27" t="s">
         <v>117</v>
       </c>
       <c r="D19" s="14" t="s">
@@ -1637,17 +1654,17 @@
       <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="28"/>
-      <c r="C20" s="26"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="10" t="s">
         <v>119</v>
       </c>
       <c r="E20" s="11"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="26"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="12" t="s">
         <v>120</v>
       </c>
@@ -1657,11 +1674,11 @@
       <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="25" t="s">
+      <c r="A22" s="25"/>
+      <c r="B22" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="27" t="s">
         <v>123</v>
       </c>
       <c r="D22" s="14" t="s">
@@ -1672,7 +1689,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>
       <c r="D23" s="14" t="s">
@@ -1681,16 +1698,16 @@
       <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="28"/>
-      <c r="C24" s="26"/>
+      <c r="C24" s="29"/>
       <c r="D24" s="14" t="s">
         <v>127</v>
       </c>
       <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="28"/>
       <c r="C25" s="14" t="s">
         <v>128</v>
@@ -1701,9 +1718,9 @@
       <c r="E25" s="11"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="28"/>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="27" t="s">
         <v>129</v>
       </c>
       <c r="D26" s="14" t="s">
@@ -1712,7 +1729,7 @@
       <c r="E26" s="11"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
+      <c r="A27" s="25"/>
       <c r="B27" s="28"/>
       <c r="C27" s="28"/>
       <c r="D27" s="14" t="s">
@@ -1721,22 +1738,22 @@
       <c r="E27" s="11"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
       <c r="D28" s="14" t="s">
         <v>132</v>
       </c>
       <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="27" t="s">
         <v>135</v>
       </c>
       <c r="D29" s="14" t="s">
@@ -1747,17 +1764,17 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="28"/>
-      <c r="C30" s="26"/>
+      <c r="C30" s="29"/>
       <c r="D30" s="14" t="s">
         <v>138</v>
       </c>
       <c r="E30" s="11"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="26"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="14" t="s">
         <v>139</v>
       </c>
@@ -1769,8 +1786,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="25" t="s">
+      <c r="A32" s="30"/>
+      <c r="B32" s="27" t="s">
         <v>142</v>
       </c>
       <c r="C32" s="14" t="s">
@@ -1782,8 +1799,8 @@
       <c r="E32" s="11"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="26"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="14" t="s">
         <v>144</v>
       </c>
@@ -1794,13 +1811,13 @@
       <c r="F33" s="16"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="27" t="s">
         <v>147</v>
       </c>
       <c r="D34" s="13" t="s">
@@ -1809,9 +1826,9 @@
       <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
       <c r="D35" s="14" t="s">
         <v>149</v>
       </c>
@@ -1832,7 +1849,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="24" t="s">
         <v>153</v>
       </c>
       <c r="B42" s="18" t="s">
@@ -1843,7 +1860,7 @@
       <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="19" t="s">
         <v>155</v>
       </c>
@@ -1852,7 +1869,7 @@
       <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="19" t="s">
         <v>156</v>
       </c>
@@ -1861,7 +1878,7 @@
       <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
+      <c r="A45" s="25"/>
       <c r="B45" s="19" t="s">
         <v>157</v>
       </c>
@@ -1869,7 +1886,7 @@
       <c r="D45" s="19"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
+      <c r="A46" s="25"/>
       <c r="B46" s="19" t="s">
         <v>158</v>
       </c>
@@ -1877,7 +1894,7 @@
       <c r="D46" s="19"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="23" t="s">
+      <c r="A47" s="24" t="s">
         <v>159</v>
       </c>
       <c r="B47" s="19" t="s">
@@ -1887,7 +1904,7 @@
       <c r="D47" s="19"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="24"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="19" t="s">
         <v>161</v>
       </c>
@@ -1895,7 +1912,7 @@
       <c r="D48" s="19"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="24"/>
+      <c r="A49" s="25"/>
       <c r="B49" s="19" t="s">
         <v>162</v>
       </c>
@@ -1903,7 +1920,7 @@
       <c r="D49" s="19"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="24"/>
+      <c r="A50" s="25"/>
       <c r="B50" s="19" t="s">
         <v>163</v>
       </c>
@@ -1911,7 +1928,7 @@
       <c r="D50" s="19"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="s">
+      <c r="A51" s="27" t="s">
         <v>164</v>
       </c>
       <c r="B51" s="19" t="s">
@@ -1921,7 +1938,7 @@
       <c r="D51" s="19"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
+      <c r="A52" s="29"/>
       <c r="B52" s="19" t="s">
         <v>142</v>
       </c>
@@ -1938,6 +1955,24 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="A16:A28"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C26:C28"/>
     <mergeCell ref="A2:A15"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C3:C4"/>
@@ -1947,24 +1982,6 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="B11:B15"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="A16:A28"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1975,8 +1992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D80F62-AD32-4D31-A959-DA3AC0FAD995}">
   <dimension ref="B2:R39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1995,27 +2012,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
-      <c r="H2" s="34" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
+      <c r="H2" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="36"/>
-      <c r="N2" s="34" t="s">
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="35"/>
+      <c r="N2" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="36"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="35"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -2027,10 +2044,10 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="33"/>
+      <c r="F3" s="32"/>
       <c r="H3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2040,10 +2057,10 @@
       <c r="J3" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="32" t="s">
+      <c r="K3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="33"/>
+      <c r="L3" s="32"/>
       <c r="N3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2053,51 +2070,51 @@
       <c r="P3" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="32" t="s">
+      <c r="Q3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="33"/>
+      <c r="R3" s="32"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="33"/>
+      <c r="F4" s="32"/>
       <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="J4" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="32" t="s">
+      <c r="K4" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="33"/>
+      <c r="L4" s="32"/>
       <c r="N4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="O4" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="P4" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="32" t="s">
+      <c r="Q4" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="R4" s="33"/>
+      <c r="R4" s="32"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -2109,8 +2126,8 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="33"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="32"/>
       <c r="H5" s="1" t="s">
         <v>39</v>
       </c>
@@ -2120,10 +2137,10 @@
       <c r="J5" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="32" t="s">
+      <c r="K5" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="33"/>
+      <c r="L5" s="32"/>
       <c r="N5" s="1" t="s">
         <v>39</v>
       </c>
@@ -2133,10 +2150,10 @@
       <c r="P5" t="s">
         <v>70</v>
       </c>
-      <c r="Q5" s="32" t="s">
+      <c r="Q5" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="R5" s="33"/>
+      <c r="R5" s="32"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -2148,21 +2165,21 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="33"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
       <c r="H6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="I6" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="J6" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="32" t="s">
+      <c r="K6" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="33"/>
+      <c r="L6" s="32"/>
       <c r="N6" s="1" t="s">
         <v>60</v>
       </c>
@@ -2172,8 +2189,8 @@
       <c r="P6" t="s">
         <v>63</v>
       </c>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="33"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="32"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -2185,21 +2202,23 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="33"/>
+      <c r="F7" s="32"/>
       <c r="H7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="I7" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="J7" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="33"/>
+      <c r="K7" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="L7" s="32"/>
       <c r="N7" s="4" t="s">
         <v>61</v>
       </c>
@@ -2209,8 +2228,8 @@
       <c r="P7" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="31"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="37"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -2222,10 +2241,10 @@
       <c r="D8" t="s">
         <v>174</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="F8" s="33"/>
+      <c r="F8" s="32"/>
       <c r="H8" s="1" t="s">
         <v>46</v>
       </c>
@@ -2235,12 +2254,12 @@
       <c r="J8" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="32" t="s">
+      <c r="K8" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="L8" s="33"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -2252,10 +2271,10 @@
       <c r="D9" t="s">
         <v>177</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="F9" s="33"/>
+      <c r="F9" s="32"/>
       <c r="H9" s="4" t="s">
         <v>36</v>
       </c>
@@ -2265,12 +2284,12 @@
       <c r="J9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="30" t="s">
+      <c r="K9" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="L9" s="31"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
+      <c r="L9" s="37"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -2282,15 +2301,15 @@
       <c r="D10" t="s">
         <v>180</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="33"/>
-      <c r="N10" s="34" t="s">
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="N10" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="36"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="35"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
@@ -2302,15 +2321,15 @@
       <c r="D11" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="31"/>
-      <c r="H11" s="34" t="s">
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
+      <c r="H11" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="36"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="35"/>
       <c r="N11" s="1" t="s">
         <v>1</v>
       </c>
@@ -2320,10 +2339,10 @@
       <c r="P11" t="s">
         <v>3</v>
       </c>
-      <c r="Q11" s="32" t="s">
+      <c r="Q11" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="R11" s="33"/>
+      <c r="R11" s="32"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H12" s="1" t="s">
@@ -2335,45 +2354,45 @@
       <c r="J12" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="32" t="s">
+      <c r="K12" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="33"/>
+      <c r="L12" s="32"/>
       <c r="N12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="O12" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="P12" t="s">
         <v>7</v>
       </c>
-      <c r="Q12" s="32" t="s">
+      <c r="Q12" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="R12" s="33"/>
+      <c r="R12" s="32"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="36"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="35"/>
       <c r="H13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I13" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="J13" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="32" t="s">
+      <c r="K13" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="L13" s="33"/>
+      <c r="L13" s="32"/>
       <c r="N13" s="1" t="s">
         <v>19</v>
       </c>
@@ -2383,10 +2402,10 @@
       <c r="P13" t="s">
         <v>20</v>
       </c>
-      <c r="Q13" s="32" t="s">
+      <c r="Q13" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="R13" s="33"/>
+      <c r="R13" s="32"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -2398,10 +2417,10 @@
       <c r="D14" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="33"/>
+      <c r="F14" s="32"/>
       <c r="H14" s="1" t="s">
         <v>51</v>
       </c>
@@ -2422,25 +2441,25 @@
       <c r="P14" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="Q14" s="30" t="s">
+      <c r="Q14" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="R14" s="31"/>
+      <c r="R14" s="37"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="33"/>
+      <c r="F15" s="32"/>
       <c r="H15" s="4" t="s">
         <v>52</v>
       </c>
@@ -2458,15 +2477,15 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="33"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -2478,22 +2497,22 @@
       <c r="D17" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-      <c r="H17" s="34" t="s">
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="H17" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="36"/>
-      <c r="N17" s="34" t="s">
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="35"/>
+      <c r="N17" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="36"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="35"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
@@ -2505,8 +2524,8 @@
       <c r="D18" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
       <c r="H18" s="1" t="s">
         <v>1</v>
       </c>
@@ -2516,10 +2535,10 @@
       <c r="J18" t="s">
         <v>3</v>
       </c>
-      <c r="K18" s="32" t="s">
+      <c r="K18" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="L18" s="33"/>
+      <c r="L18" s="32"/>
       <c r="N18" s="1" t="s">
         <v>1</v>
       </c>
@@ -2529,10 +2548,10 @@
       <c r="P18" t="s">
         <v>3</v>
       </c>
-      <c r="Q18" s="32" t="s">
+      <c r="Q18" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="R18" s="33"/>
+      <c r="R18" s="32"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
@@ -2544,36 +2563,36 @@
       <c r="D19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="31"/>
+      <c r="F19" s="37"/>
       <c r="H19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I19" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="J19" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="32" t="s">
+      <c r="K19" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="L19" s="33"/>
+      <c r="L19" s="32"/>
       <c r="N19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="O19" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="P19" t="s">
         <v>7</v>
       </c>
-      <c r="Q19" s="32" t="s">
+      <c r="Q19" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="R19" s="33"/>
+      <c r="R19" s="32"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H20" s="1" t="s">
@@ -2585,30 +2604,30 @@
       <c r="J20" t="s">
         <v>57</v>
       </c>
-      <c r="K20" s="32" t="s">
+      <c r="K20" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="L20" s="33"/>
+      <c r="L20" s="32"/>
       <c r="N20" s="1" t="s">
         <v>44</v>
       </c>
       <c r="O20" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="P20" t="s">
         <v>68</v>
       </c>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="33"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="32"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="35"/>
       <c r="H21" s="1" t="s">
         <v>60</v>
       </c>
@@ -2618,23 +2637,23 @@
       <c r="J21" t="s">
         <v>63</v>
       </c>
-      <c r="K21" s="32" t="s">
+      <c r="K21" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="L21" s="33"/>
+      <c r="L21" s="32"/>
       <c r="N21" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="O21" s="5" t="s">
-        <v>6</v>
+      <c r="O21" t="s">
+        <v>183</v>
       </c>
       <c r="P21" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="Q21" s="30" t="s">
+      <c r="Q21" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="R21" s="31"/>
+      <c r="R21" s="37"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
@@ -2646,10 +2665,10 @@
       <c r="D22" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="32" t="s">
+      <c r="E22" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="33"/>
+      <c r="F22" s="32"/>
       <c r="H22" s="1" t="s">
         <v>61</v>
       </c>
@@ -2659,25 +2678,25 @@
       <c r="J22" t="s">
         <v>64</v>
       </c>
-      <c r="K22" s="32" t="s">
+      <c r="K22" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="L22" s="33"/>
+      <c r="L22" s="32"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="33"/>
+      <c r="F23" s="32"/>
       <c r="H23" s="1" t="s">
         <v>58</v>
       </c>
@@ -2687,10 +2706,10 @@
       <c r="J23" t="s">
         <v>59</v>
       </c>
-      <c r="K23" s="32" t="s">
+      <c r="K23" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="L23" s="33"/>
+      <c r="L23" s="32"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
@@ -2702,10 +2721,10 @@
       <c r="D24" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="33"/>
+      <c r="F24" s="32"/>
       <c r="H24" s="1" t="s">
         <v>171</v>
       </c>
@@ -2715,8 +2734,8 @@
       <c r="J24" t="s">
         <v>180</v>
       </c>
-      <c r="K24" s="32"/>
-      <c r="L24" s="33"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="32"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
@@ -2728,10 +2747,10 @@
       <c r="D25" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="33"/>
+      <c r="F25" s="32"/>
       <c r="H25" s="4" t="s">
         <v>172</v>
       </c>
@@ -2741,8 +2760,8 @@
       <c r="J25" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="K25" s="30"/>
-      <c r="L25" s="31"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="37"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
@@ -2754,8 +2773,8 @@
       <c r="D26" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="32"/>
-      <c r="F26" s="33"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
@@ -2767,19 +2786,19 @@
       <c r="D27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="31"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="36"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="35"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
@@ -2791,55 +2810,55 @@
       <c r="D30" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="32" t="s">
+      <c r="E30" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="33"/>
+      <c r="F30" s="32"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="32"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="D32" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="32" t="s">
+      <c r="E32" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="32"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="D33" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="32" t="s">
+      <c r="E33" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="F33" s="33"/>
+      <c r="F33" s="32"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
@@ -2851,8 +2870,8 @@
       <c r="D34" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="32"/>
-      <c r="F34" s="33"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="32"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
@@ -2864,8 +2883,8 @@
       <c r="D35" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="33"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="32"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
@@ -2877,8 +2896,8 @@
       <c r="D36" t="s">
         <v>180</v>
       </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="33"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="32"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
@@ -2890,15 +2909,71 @@
       <c r="D37" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="E37" s="30"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="37"/>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="K39" s="32"/>
-      <c r="L39" s="32"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="72">
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="N10:R10"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q6:R6"/>
     <mergeCell ref="K39:L39"/>
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="K19:L19"/>
@@ -2914,63 +2989,7 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="N10:R10"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E11:F11"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K22:L22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2982,8 +3001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A16CED-1914-426A-8275-7025C555F9C2}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2994,13 +3013,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="23" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3012,7 +3031,48 @@
         <v>13456</v>
       </c>
       <c r="C2" s="2">
-        <v>3</v>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447FBABE-C614-4DFE-8D67-B03DA27B8FBE}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>20201111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>